<commit_message>
added optmization logics for obstacles
</commit_message>
<xml_diff>
--- a/model/a-multiple-objective-optimization-model-for-community-covid-19-sampling-site_CN.xlsx
+++ b/model/a-multiple-objective-optimization-model-for-community-covid-19-sampling-site_CN.xlsx
@@ -15,6 +15,10 @@
     <sheet name="小区核算采样选址优化" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="O1_X">小区核算采样选址优化!$B$29</definedName>
+    <definedName name="O1_Y">小区核算采样选址优化!$C$29</definedName>
+    <definedName name="O2_X">小区核算采样选址优化!$B$30</definedName>
+    <definedName name="O2_Y">小区核算采样选址优化!$C$30</definedName>
     <definedName name="p_w">小区核算采样选址优化!$F$17</definedName>
     <definedName name="x_o">小区核算采样选址优化!$G$17</definedName>
     <definedName name="y_o">小区核算采样选址优化!$H$17</definedName>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>1, 2</t>
   </si>
@@ -75,12 +79,47 @@
   <si>
     <t>3,4</t>
   </si>
+  <si>
+    <t>3,0</t>
+  </si>
+  <si>
+    <t>6,8</t>
+  </si>
+  <si>
+    <t>Obstacles</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s.t.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> min(D(S, obstacle_i)) &gt; 0</t>
+    </r>
+  </si>
+  <si>
+    <t>Available Sites Matrix</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +150,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -155,6 +216,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -168,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -177,6 +250,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -195,7 +274,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$17" inc="5" max="100" page="10" val="50"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$17" inc="5" max="100" page="10" val="60"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -293,16 +372,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590549</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -311,7 +390,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6076949" y="2371726"/>
+          <a:off x="5200649" y="2362201"/>
           <a:ext cx="4286251" cy="276224"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -609,7 +688,7 @@
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>50</a:t>
+            <a:t>60</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -883,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P25"/>
+  <dimension ref="A3:S48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +977,7 @@
     <col min="7" max="7" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -922,7 +1001,7 @@
       </c>
       <c r="I3">
         <f>ABS(x_o-B18)+ABS(y_o-C18)+ABS(x_o-B19)+ABS(y_o-C19)+ABS(x_o-B20)+ABS(y_o-C20)+ABS(x_o-B21)+ABS(y_o-C21)+ABS(x_o-B22)+ABS(y_o-C22)+ABS(x_o-B23)+ABS(y_o-C23)+ABS(x_o-B24)+ABS(y_o-C24)+ABS(x_o-B25)+ABS(y_o-C25)-p_w*(ABS(x_o-D18)+ABS(y_o-E18))</f>
-        <v>-296</v>
+        <v>-366</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -946,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -955,7 +1034,9 @@
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -964,28 +1045,28 @@
       </c>
       <c r="J4" s="7">
         <f t="dataTable" ref="J4:P12" dt2D="1" dtr="1" r1="G17" r2="H17" ca="1"/>
-        <v>-296</v>
+        <v>-366</v>
       </c>
       <c r="K4" s="7">
+        <v>-314</v>
+      </c>
+      <c r="L4" s="7">
+        <v>-256</v>
+      </c>
+      <c r="M4" s="7">
+        <v>-196</v>
+      </c>
+      <c r="N4" s="7">
         <v>-254</v>
       </c>
-      <c r="L4" s="7">
-        <v>-206</v>
-      </c>
-      <c r="M4" s="7">
-        <v>-156</v>
-      </c>
-      <c r="N4" s="7">
-        <v>-204</v>
-      </c>
       <c r="O4" s="7">
-        <v>-250</v>
+        <v>-310</v>
       </c>
       <c r="P4" s="7">
-        <v>-292</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1000,28 +1081,28 @@
         <v>1</v>
       </c>
       <c r="J5" s="7">
-        <v>-252</v>
+        <v>-312</v>
       </c>
       <c r="K5" s="7">
-        <v>-210</v>
+        <v>-260</v>
       </c>
       <c r="L5" s="7">
-        <v>-162</v>
+        <v>-202</v>
       </c>
       <c r="M5" s="7">
-        <v>-112</v>
+        <v>-142</v>
       </c>
       <c r="N5" s="7">
-        <v>-160</v>
+        <v>-200</v>
       </c>
       <c r="O5" s="7">
-        <v>-206</v>
+        <v>-256</v>
       </c>
       <c r="P5" s="7">
-        <v>-248</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1040,28 +1121,28 @@
         <v>2</v>
       </c>
       <c r="J6" s="7">
-        <v>-208</v>
+        <v>-258</v>
       </c>
       <c r="K6" s="7">
-        <v>-166</v>
+        <v>-206</v>
       </c>
       <c r="L6" s="7">
-        <v>-118</v>
+        <v>-148</v>
       </c>
       <c r="M6" s="7">
-        <v>-68</v>
+        <v>-88</v>
       </c>
       <c r="N6" s="7">
-        <v>-116</v>
+        <v>-146</v>
       </c>
       <c r="O6" s="7">
-        <v>-162</v>
+        <v>-202</v>
       </c>
       <c r="P6" s="7">
-        <v>-204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1076,28 +1157,28 @@
         <v>3</v>
       </c>
       <c r="J7" s="7">
-        <v>-160</v>
+        <v>-200</v>
       </c>
       <c r="K7" s="7">
-        <v>-118</v>
+        <v>-148</v>
       </c>
       <c r="L7" s="7">
-        <v>-70</v>
+        <v>-90</v>
       </c>
       <c r="M7" s="7">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="N7" s="7">
-        <v>-68</v>
+        <v>-88</v>
       </c>
       <c r="O7" s="7">
-        <v>-114</v>
+        <v>-144</v>
       </c>
       <c r="P7" s="7">
-        <v>-156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1116,28 +1197,28 @@
         <v>4</v>
       </c>
       <c r="J8" s="7">
-        <v>-112</v>
+        <v>-142</v>
       </c>
       <c r="K8" s="7">
-        <v>-70</v>
+        <v>-90</v>
       </c>
       <c r="L8" s="7">
-        <v>-22</v>
+        <v>-32</v>
       </c>
       <c r="M8" s="7">
         <v>28</v>
       </c>
       <c r="N8" s="7">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="O8" s="7">
-        <v>-66</v>
+        <v>-86</v>
       </c>
       <c r="P8" s="7">
-        <v>-108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1152,28 +1233,28 @@
         <v>5</v>
       </c>
       <c r="J9" s="7">
-        <v>-160</v>
+        <v>-200</v>
       </c>
       <c r="K9" s="7">
-        <v>-118</v>
+        <v>-148</v>
       </c>
       <c r="L9" s="7">
-        <v>-70</v>
+        <v>-90</v>
       </c>
       <c r="M9" s="7">
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="N9" s="7">
-        <v>-68</v>
+        <v>-88</v>
       </c>
       <c r="O9" s="7">
-        <v>-114</v>
+        <v>-144</v>
       </c>
       <c r="P9" s="7">
-        <v>-156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1192,28 +1273,28 @@
         <v>6</v>
       </c>
       <c r="J10" s="7">
-        <v>-208</v>
+        <v>-258</v>
       </c>
       <c r="K10" s="7">
-        <v>-166</v>
+        <v>-206</v>
       </c>
       <c r="L10" s="7">
-        <v>-118</v>
+        <v>-148</v>
       </c>
       <c r="M10" s="7">
-        <v>-68</v>
+        <v>-88</v>
       </c>
       <c r="N10" s="7">
-        <v>-116</v>
+        <v>-146</v>
       </c>
       <c r="O10" s="7">
-        <v>-162</v>
+        <v>-202</v>
       </c>
       <c r="P10" s="7">
-        <v>-204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1228,28 +1309,28 @@
         <v>7</v>
       </c>
       <c r="J11" s="7">
-        <v>-252</v>
+        <v>-312</v>
       </c>
       <c r="K11" s="7">
-        <v>-210</v>
+        <v>-260</v>
       </c>
       <c r="L11" s="7">
-        <v>-162</v>
+        <v>-202</v>
       </c>
       <c r="M11" s="7">
-        <v>-112</v>
+        <v>-142</v>
       </c>
       <c r="N11" s="7">
-        <v>-160</v>
+        <v>-200</v>
       </c>
       <c r="O11" s="7">
-        <v>-206</v>
+        <v>-256</v>
       </c>
       <c r="P11" s="7">
-        <v>-248</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-308</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1261,33 +1342,35 @@
         <v>7</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="8" t="s">
+        <v>16</v>
+      </c>
       <c r="I12">
         <v>8</v>
       </c>
       <c r="J12" s="7">
-        <v>-296</v>
+        <v>-366</v>
       </c>
       <c r="K12" s="7">
+        <v>-314</v>
+      </c>
+      <c r="L12" s="7">
+        <v>-256</v>
+      </c>
+      <c r="M12" s="7">
+        <v>-196</v>
+      </c>
+      <c r="N12" s="7">
         <v>-254</v>
       </c>
-      <c r="L12" s="7">
-        <v>-206</v>
-      </c>
-      <c r="M12" s="7">
-        <v>-156</v>
-      </c>
-      <c r="N12" s="7">
-        <v>-204</v>
-      </c>
       <c r="O12" s="7">
-        <v>-250</v>
+        <v>-310</v>
       </c>
       <c r="P12" s="7">
-        <v>-292</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>-362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I15">
         <f>MIN(ABS(x_o-B18)+ABS(y_o-C18), ABS(x_o-B19)+ABS(y_o-C19), ABS(x_o-B20)+ABS(y_o-C20), ABS(x_o-B21)+ABS(y_o-C21), ABS(x_o-B22)+ABS(y_o-C22), ABS(x_o-B23)+ABS(y_o-C23), ABS(x_o-B24)+ABS(y_o-C24), ABS(x_o-B25)+ABS(y_o-C25))</f>
         <v>2</v>
@@ -1314,7 +1397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
@@ -1357,6 +1440,7 @@
       <c r="P16" s="7">
         <v>3</v>
       </c>
+      <c r="S16" s="12"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
@@ -1372,7 +1456,7 @@
         <v>10</v>
       </c>
       <c r="F17">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1657,9 +1741,631 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="10"/>
+      <c r="I27">
+        <f>IF(MIN(ABS(x_o-O1_X)+ABS(y_o-O1_Y), ABS(x_o-O2_X)+ABS(y_o-O2_Y)) &gt; 0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>4</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="P27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="dataTable" ref="J28:P36" dt2D="1" dtr="1" r1="G17" r2="H17" ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="7">
+        <v>1</v>
+      </c>
+      <c r="L28" s="7">
+        <v>1</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
+        <v>1</v>
+      </c>
+      <c r="O28" s="7">
+        <v>1</v>
+      </c>
+      <c r="P28" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" s="11">
+        <v>3</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" s="7">
+        <v>1</v>
+      </c>
+      <c r="K29" s="7">
+        <v>1</v>
+      </c>
+      <c r="L29" s="7">
+        <v>1</v>
+      </c>
+      <c r="M29" s="7">
+        <v>1</v>
+      </c>
+      <c r="N29" s="7">
+        <v>1</v>
+      </c>
+      <c r="O29" s="7">
+        <v>1</v>
+      </c>
+      <c r="P29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <v>6</v>
+      </c>
+      <c r="C30" s="11">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30" s="7">
+        <v>1</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+      <c r="L30" s="7">
+        <v>1</v>
+      </c>
+      <c r="M30" s="7">
+        <v>1</v>
+      </c>
+      <c r="N30" s="7">
+        <v>1</v>
+      </c>
+      <c r="O30" s="7">
+        <v>1</v>
+      </c>
+      <c r="P30" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31" s="7">
+        <v>1</v>
+      </c>
+      <c r="K31" s="7">
+        <v>1</v>
+      </c>
+      <c r="L31" s="7">
+        <v>1</v>
+      </c>
+      <c r="M31" s="7">
+        <v>1</v>
+      </c>
+      <c r="N31" s="7">
+        <v>1</v>
+      </c>
+      <c r="O31" s="7">
+        <v>1</v>
+      </c>
+      <c r="P31" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="I32">
+        <v>4</v>
+      </c>
+      <c r="J32" s="7">
+        <v>1</v>
+      </c>
+      <c r="K32" s="7">
+        <v>1</v>
+      </c>
+      <c r="L32" s="7">
+        <v>1</v>
+      </c>
+      <c r="M32" s="7">
+        <v>1</v>
+      </c>
+      <c r="N32" s="7">
+        <v>1</v>
+      </c>
+      <c r="O32" s="7">
+        <v>1</v>
+      </c>
+      <c r="P32" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="I33">
+        <v>5</v>
+      </c>
+      <c r="J33" s="7">
+        <v>1</v>
+      </c>
+      <c r="K33" s="7">
+        <v>1</v>
+      </c>
+      <c r="L33" s="7">
+        <v>1</v>
+      </c>
+      <c r="M33" s="7">
+        <v>1</v>
+      </c>
+      <c r="N33" s="7">
+        <v>1</v>
+      </c>
+      <c r="O33" s="7">
+        <v>1</v>
+      </c>
+      <c r="P33" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="I34">
+        <v>6</v>
+      </c>
+      <c r="J34" s="7">
+        <v>1</v>
+      </c>
+      <c r="K34" s="7">
+        <v>1</v>
+      </c>
+      <c r="L34" s="7">
+        <v>1</v>
+      </c>
+      <c r="M34" s="7">
+        <v>1</v>
+      </c>
+      <c r="N34" s="7">
+        <v>1</v>
+      </c>
+      <c r="O34" s="7">
+        <v>1</v>
+      </c>
+      <c r="P34" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>7</v>
+      </c>
+      <c r="J35" s="7">
+        <v>1</v>
+      </c>
+      <c r="K35" s="7">
+        <v>1</v>
+      </c>
+      <c r="L35" s="7">
+        <v>1</v>
+      </c>
+      <c r="M35" s="7">
+        <v>1</v>
+      </c>
+      <c r="N35" s="7">
+        <v>1</v>
+      </c>
+      <c r="O35" s="7">
+        <v>1</v>
+      </c>
+      <c r="P35" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1</v>
+      </c>
+      <c r="K36" s="7">
+        <v>1</v>
+      </c>
+      <c r="L36" s="7">
+        <v>1</v>
+      </c>
+      <c r="M36" s="7">
+        <v>1</v>
+      </c>
+      <c r="N36" s="7">
+        <v>1</v>
+      </c>
+      <c r="O36" s="7">
+        <v>1</v>
+      </c>
+      <c r="P36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J38" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>2</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <v>4</v>
+      </c>
+      <c r="O39">
+        <v>5</v>
+      </c>
+      <c r="P39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" s="13">
+        <f>J16*J28</f>
+        <v>2</v>
+      </c>
+      <c r="K40" s="13">
+        <f t="shared" ref="K40:P40" si="0">K16*K28</f>
+        <v>1</v>
+      </c>
+      <c r="L40" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O40" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P40" s="13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41" s="13">
+        <f t="shared" ref="J41:P41" si="1">J17*J29</f>
+        <v>2</v>
+      </c>
+      <c r="K41" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L41" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M41" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N41" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O41" s="13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P41" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42" s="13">
+        <f t="shared" ref="J42:P42" si="2">J18*J30</f>
+        <v>1</v>
+      </c>
+      <c r="K42" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L42" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M42" s="13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N42" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O42" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P42" s="13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="J43" s="13">
+        <f t="shared" ref="J43:P43" si="3">J19*J31</f>
+        <v>2</v>
+      </c>
+      <c r="K43" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L43" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="M43" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N43" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="O43" s="13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P43" s="13">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>4</v>
+      </c>
+      <c r="J44" s="13">
+        <f t="shared" ref="J44:P44" si="4">J20*J32</f>
+        <v>1</v>
+      </c>
+      <c r="K44" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="M44" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="13">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O44" s="13">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="P44" s="13">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>5</v>
+      </c>
+      <c r="J45" s="13">
+        <f t="shared" ref="J45:P45" si="5">J21*J33</f>
+        <v>2</v>
+      </c>
+      <c r="K45" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="L45" s="13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="M45" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N45" s="13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="O45" s="13">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P45" s="13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>6</v>
+      </c>
+      <c r="J46" s="13">
+        <f t="shared" ref="J46:P46" si="6">J22*J34</f>
+        <v>1</v>
+      </c>
+      <c r="K46" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M46" s="13">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="N46" s="13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O46" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="13">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>7</v>
+      </c>
+      <c r="J47" s="13">
+        <f t="shared" ref="J47:P47" si="7">J23*J35</f>
+        <v>2</v>
+      </c>
+      <c r="K47" s="13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L47" s="13">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="M47" s="13">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N47" s="13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="O47" s="13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P47" s="13">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>8</v>
+      </c>
+      <c r="J48" s="13">
+        <f t="shared" ref="J48:P48" si="8">J24*J36</f>
+        <v>3</v>
+      </c>
+      <c r="K48" s="13">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="L48" s="13">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="M48" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="N48" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O48" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="P48" s="13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J4:P12">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1671,6 +2377,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:P24">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:P36">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J40:P48">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>